<commit_message>
CORRECTED METHOD IN ACTION MAP
</commit_message>
<xml_diff>
--- a/Action Map3.xlsx
+++ b/Action Map3.xlsx
@@ -291,9 +291,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -306,6 +303,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,457 +634,457 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="10"/>
+      <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="10"/>
+      <c r="B20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="10"/>
+      <c r="B22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="10"/>
+      <c r="B26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="B27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="10"/>
+      <c r="B28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="A30" s="10"/>
+      <c r="B30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="8" t="s">
+      <c r="A31" s="10"/>
+      <c r="B31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="10"/>
+      <c r="B32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="10"/>
+      <c r="B34" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A36" s="10"/>
+      <c r="B36" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="C36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
     <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5" t="s">
+      <c r="A37" s="10"/>
+      <c r="B37" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="9" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A35:A37"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A14"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="A21:A26"/>
     <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A35:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>